<commit_message>
Collect 0418 small dataset
</commit_message>
<xml_diff>
--- a/graph/231116_231117.xlsx
+++ b/graph/231116_231117.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Experiment\graph\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{9748E0D5-B8B5-4749-89FE-1C4DB87667D5}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{C4549794-C11B-4131-A2C9-26C64FFA4DB4}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="0" windowWidth="22260" windowHeight="12645" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -349,7 +349,7 @@
                   <c:v>1</c:v>
                 </c:pt>
                 <c:pt idx="4">
-                  <c:v>1.04</c:v>
+                  <c:v>0.91</c:v>
                 </c:pt>
                 <c:pt idx="5">
                   <c:v>1</c:v>
@@ -511,7 +511,7 @@
                   <c:v>1.44</c:v>
                 </c:pt>
                 <c:pt idx="4">
-                  <c:v>0.99</c:v>
+                  <c:v>1.1399999999999999</c:v>
                 </c:pt>
                 <c:pt idx="5">
                   <c:v>1.33</c:v>
@@ -2930,7 +2930,7 @@
   <dimension ref="D5:F31"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="T3" sqref="T3"/>
+      <selection activeCell="F12" sqref="F12"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15.75" x14ac:dyDescent="0.25"/>
@@ -3005,10 +3005,10 @@
         <v>8</v>
       </c>
       <c r="E11">
-        <v>1.04</v>
+        <v>0.91</v>
       </c>
       <c r="F11">
-        <v>0.99</v>
+        <v>1.1399999999999999</v>
       </c>
     </row>
     <row r="12" spans="4:6" x14ac:dyDescent="0.25">

</xml_diff>